<commit_message>
Succeffely added functions to caculate data for City, Uni, Faculty, graduation year,
</commit_message>
<xml_diff>
--- a/uploads/example_data.xlsx
+++ b/uploads/example_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\MSPdata\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\mysitemsp\MSPdata\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="472">
   <si>
     <t>Customer ID</t>
   </si>
@@ -983,9 +983,6 @@
     <t>Alexaindria University</t>
   </si>
   <si>
-    <t>Ahram Canadian University</t>
-  </si>
-  <si>
     <t>south sinai university</t>
   </si>
   <si>
@@ -1290,6 +1287,159 @@
   </si>
   <si>
     <t>Intermediat</t>
+  </si>
+  <si>
+    <t>instagram 1</t>
+  </si>
+  <si>
+    <t>instagram 2</t>
+  </si>
+  <si>
+    <t>instagram 3</t>
+  </si>
+  <si>
+    <t>instagram 4</t>
+  </si>
+  <si>
+    <t>instagram 5</t>
+  </si>
+  <si>
+    <t>instagram 6</t>
+  </si>
+  <si>
+    <t>instagram 7</t>
+  </si>
+  <si>
+    <t>instagram 8</t>
+  </si>
+  <si>
+    <t>instagram 9</t>
+  </si>
+  <si>
+    <t>instagram 10</t>
+  </si>
+  <si>
+    <t>instagram 11</t>
+  </si>
+  <si>
+    <t>instagram 12</t>
+  </si>
+  <si>
+    <t>instagram 13</t>
+  </si>
+  <si>
+    <t>instagram 14</t>
+  </si>
+  <si>
+    <t>instagram 15</t>
+  </si>
+  <si>
+    <t>facebook1</t>
+  </si>
+  <si>
+    <t>facebook2</t>
+  </si>
+  <si>
+    <t>facebook3</t>
+  </si>
+  <si>
+    <t>facebook4</t>
+  </si>
+  <si>
+    <t>facebook5</t>
+  </si>
+  <si>
+    <t>facebook6</t>
+  </si>
+  <si>
+    <t>facebook7</t>
+  </si>
+  <si>
+    <t>facebook8</t>
+  </si>
+  <si>
+    <t>facebook9</t>
+  </si>
+  <si>
+    <t>facebook10</t>
+  </si>
+  <si>
+    <t>facebook11</t>
+  </si>
+  <si>
+    <t>facebook12</t>
+  </si>
+  <si>
+    <t>facebook13</t>
+  </si>
+  <si>
+    <t>facebook14</t>
+  </si>
+  <si>
+    <t>facebook15</t>
+  </si>
+  <si>
+    <t>yes1</t>
+  </si>
+  <si>
+    <t>yes3</t>
+  </si>
+  <si>
+    <t>yes5</t>
+  </si>
+  <si>
+    <t>yes7</t>
+  </si>
+  <si>
+    <t>yes8</t>
+  </si>
+  <si>
+    <t>yes9</t>
+  </si>
+  <si>
+    <t>yes10</t>
+  </si>
+  <si>
+    <t>yes11</t>
+  </si>
+  <si>
+    <t>yes12</t>
+  </si>
+  <si>
+    <t>yes13</t>
+  </si>
+  <si>
+    <t>yes14</t>
+  </si>
+  <si>
+    <t>Scientific</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Computer science</t>
+  </si>
+  <si>
+    <t>Business-related</t>
+  </si>
+  <si>
+    <t>Medical</t>
+  </si>
+  <si>
+    <t>Faculty of Agriculture</t>
+  </si>
+  <si>
+    <t>Faculty of Science</t>
+  </si>
+  <si>
+    <t>alexnadria</t>
+  </si>
+  <si>
+    <t>Alexandria</t>
   </si>
 </sst>
 </file>
@@ -1419,6 +1569,215 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>222</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>222</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Control 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>222</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>222</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Control 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>222</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>222</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Control 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>222</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>222</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Control 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1683,14 +2042,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:KQ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:KQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
-      <selection activeCell="BE9" sqref="BE9"/>
+    <sheetView tabSelected="1" topLeftCell="DI1" workbookViewId="0">
+      <selection activeCell="DQ3" sqref="DQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="53" max="53" width="21" customWidth="1"/>
+    <col min="61" max="61" width="23.42578125" customWidth="1"/>
+    <col min="69" max="69" width="26.5703125" customWidth="1"/>
+    <col min="173" max="173" width="24.5703125" customWidth="1"/>
+    <col min="177" max="177" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="9" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:303" s="8" customFormat="1" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2611,37 +2980,37 @@
         <v>311</v>
       </c>
       <c r="BI2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="BM2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="BQ2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="BU2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="BY2" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="CC2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="CG2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="CK2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="CO2" t="s">
         <v>312</v>
       </c>
       <c r="CS2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="CW2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="DA2" t="s">
         <v>312</v>
@@ -2650,7 +3019,7 @@
         <v>34241</v>
       </c>
       <c r="DI2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="DM2" t="s">
         <v>311</v>
@@ -2659,34 +3028,46 @@
         <v>2016</v>
       </c>
       <c r="DU2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="DY2" t="s">
         <v>312</v>
       </c>
       <c r="EC2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="EG2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="EK2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="ES2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="EW2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="FA2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="FI2" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="FM2" t="s">
         <v>420</v>
       </c>
-      <c r="FM2" t="s">
+      <c r="FQ2" t="s">
         <v>421</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>436</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>451</v>
+      </c>
+      <c r="HO2" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="3" spans="1:303" x14ac:dyDescent="0.25">
@@ -2696,35 +3077,35 @@
       <c r="BE3" t="s">
         <v>312</v>
       </c>
-      <c r="BI3" t="s">
-        <v>391</v>
+      <c r="BI3" s="13" t="s">
+        <v>315</v>
       </c>
       <c r="BM3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BQ3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="BU3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BY3" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="CC3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="CG3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="CK3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="CO3" t="s">
         <v>311</v>
       </c>
       <c r="CS3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="CW3">
         <v>6</v>
@@ -2736,7 +3117,7 @@
         <v>34240</v>
       </c>
       <c r="DI3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="DM3" t="s">
         <v>311</v>
@@ -2745,34 +3126,46 @@
         <v>2017</v>
       </c>
       <c r="DU3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="DY3" t="s">
         <v>311</v>
       </c>
       <c r="EC3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="EG3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="EK3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="ES3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="EW3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="FA3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="FI3" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="FM3" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="FM3" s="13" t="s">
-        <v>421</v>
+      <c r="FQ3" t="s">
+        <v>422</v>
+      </c>
+      <c r="FU3" t="s">
+        <v>437</v>
+      </c>
+      <c r="FY3" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="HO3" s="13" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="4" spans="1:303" x14ac:dyDescent="0.25">
@@ -2783,37 +3176,37 @@
         <v>313</v>
       </c>
       <c r="BI4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="BM4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="BQ4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="BU4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="BY4" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="CC4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="CG4" t="s">
         <v>312</v>
       </c>
       <c r="CK4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="CO4" t="s">
         <v>312</v>
       </c>
       <c r="CS4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CW4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="DA4" t="s">
         <v>312</v>
@@ -2822,7 +3215,7 @@
         <v>34239</v>
       </c>
       <c r="DI4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="DM4" t="s">
         <v>311</v>
@@ -2831,34 +3224,46 @@
         <v>2016</v>
       </c>
       <c r="DU4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="DY4" t="s">
         <v>312</v>
       </c>
       <c r="EC4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="EG4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="EK4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="ES4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="EW4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="FA4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="FI4" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="FM4" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="FM4" s="13" t="s">
-        <v>421</v>
+      <c r="FQ4" t="s">
+        <v>423</v>
+      </c>
+      <c r="FU4" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="FY4" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="HO4" s="13" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="5" spans="1:303" x14ac:dyDescent="0.25">
@@ -2868,26 +3273,26 @@
       <c r="BE5" t="s">
         <v>311</v>
       </c>
-      <c r="BI5" t="s">
-        <v>316</v>
-      </c>
-      <c r="BQ5" t="s">
-        <v>323</v>
+      <c r="BI5" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="BQ5" s="13" t="s">
+        <v>322</v>
       </c>
       <c r="BU5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="BY5" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="CC5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="CG5" t="s">
         <v>312</v>
       </c>
       <c r="CK5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="CO5" t="s">
         <v>311</v>
@@ -2905,7 +3310,7 @@
         <v>34238</v>
       </c>
       <c r="DI5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="DM5" t="s">
         <v>311</v>
@@ -2914,34 +3319,46 @@
         <v>2018</v>
       </c>
       <c r="DU5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="DY5" t="s">
         <v>311</v>
       </c>
       <c r="EC5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="EG5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="EK5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="ES5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="EW5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="FA5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="FI5" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="FM5" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="FM5" s="13" t="s">
-        <v>421</v>
+      <c r="FQ5" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="FU5" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="FY5" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="HO5" s="13" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="6" spans="1:303" x14ac:dyDescent="0.25">
@@ -2951,26 +3368,26 @@
       <c r="BE6" t="s">
         <v>314</v>
       </c>
-      <c r="BI6" t="s">
-        <v>315</v>
+      <c r="BI6" s="13" t="s">
+        <v>316</v>
       </c>
       <c r="BQ6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="BU6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="BY6" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="CC6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="CG6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="CK6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="CO6" t="s">
         <v>312</v>
@@ -2979,7 +3396,7 @@
         <v>312</v>
       </c>
       <c r="CW6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="DA6" t="s">
         <v>312</v>
@@ -2988,46 +3405,58 @@
         <v>34237</v>
       </c>
       <c r="DI6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="DM6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="DQ6">
         <v>2020</v>
       </c>
       <c r="DU6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="DY6" t="s">
         <v>312</v>
       </c>
       <c r="EC6" t="s">
+        <v>390</v>
+      </c>
+      <c r="EG6" t="s">
+        <v>384</v>
+      </c>
+      <c r="EK6" t="s">
+        <v>407</v>
+      </c>
+      <c r="EO6" t="s">
         <v>391</v>
       </c>
-      <c r="EG6" t="s">
-        <v>385</v>
-      </c>
-      <c r="EK6" t="s">
-        <v>408</v>
-      </c>
-      <c r="EO6" t="s">
-        <v>392</v>
-      </c>
       <c r="ES6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="EW6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="FA6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="FI6" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="FM6" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="FM6" s="13" t="s">
-        <v>421</v>
+      <c r="FQ6" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="FU6" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="FY6" s="13" t="s">
+        <v>453</v>
+      </c>
+      <c r="HO6" s="13" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="1:303" x14ac:dyDescent="0.25">
@@ -3037,32 +3466,32 @@
       <c r="BE7" t="s">
         <v>312</v>
       </c>
-      <c r="BI7" t="s">
-        <v>317</v>
+      <c r="BI7" s="13" t="s">
+        <v>316</v>
       </c>
       <c r="BQ7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="BU7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="BY7" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="CC7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="CG7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="CK7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="CO7" t="s">
         <v>311</v>
       </c>
       <c r="CS7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CW7">
         <v>3</v>
@@ -3074,7 +3503,7 @@
         <v>34236</v>
       </c>
       <c r="DI7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="DM7" t="s">
         <v>311</v>
@@ -3083,37 +3512,49 @@
         <v>2021</v>
       </c>
       <c r="DU7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="DY7" t="s">
         <v>311</v>
       </c>
       <c r="EC7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="EG7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="EK7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="EO7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="ES7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="EW7" t="s">
+        <v>418</v>
+      </c>
+      <c r="FA7" t="s">
+        <v>400</v>
+      </c>
+      <c r="FI7" s="12" t="s">
         <v>419</v>
       </c>
-      <c r="FA7" t="s">
-        <v>401</v>
-      </c>
-      <c r="FI7" s="12" t="s">
+      <c r="FM7" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="FM7" s="13" t="s">
-        <v>421</v>
+      <c r="FQ7" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="FU7" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="FY7" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="HO7" s="13" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="8" spans="1:303" x14ac:dyDescent="0.25">
@@ -3123,24 +3564,24 @@
       <c r="BE8" t="s">
         <v>311</v>
       </c>
-      <c r="BI8" t="s">
-        <v>319</v>
-      </c>
-      <c r="BQ8" t="s">
-        <v>326</v>
+      <c r="BI8" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="BQ8" s="13" t="s">
+        <v>323</v>
       </c>
       <c r="BU8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BY8" s="9"/>
       <c r="CC8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="CG8" t="s">
         <v>312</v>
       </c>
       <c r="CK8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="CO8" t="s">
         <v>312</v>
@@ -3160,41 +3601,53 @@
       <c r="DM8" t="s">
         <v>312</v>
       </c>
-      <c r="DQ8">
-        <v>2017</v>
+      <c r="DQ8" s="13">
+        <v>2021</v>
       </c>
       <c r="DU8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="DY8" t="s">
         <v>312</v>
       </c>
       <c r="EC8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="EG8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="EK8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="EO8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="ES8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="EW8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="FA8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="FI8" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="FM8" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="FM8" s="13" t="s">
-        <v>421</v>
+      <c r="FQ8" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="FU8" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="FY8" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="HO8" s="13" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:303" x14ac:dyDescent="0.25">
@@ -3204,26 +3657,26 @@
       <c r="BE9" t="s">
         <v>313</v>
       </c>
-      <c r="BI9" t="s">
-        <v>318</v>
-      </c>
-      <c r="BQ9" t="s">
-        <v>327</v>
+      <c r="BI9" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="BQ9" s="13" t="s">
+        <v>323</v>
       </c>
       <c r="BU9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="BY9" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="CC9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="CG9" t="s">
         <v>312</v>
       </c>
       <c r="CK9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="CO9" t="s">
         <v>311</v>
@@ -3232,7 +3685,7 @@
         <v>312</v>
       </c>
       <c r="CW9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="DA9" t="s">
         <v>311</v>
@@ -3241,46 +3694,606 @@
         <v>34234</v>
       </c>
       <c r="DI9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="DM9" t="s">
-        <v>372</v>
-      </c>
-      <c r="DQ9">
-        <v>2025</v>
+        <v>371</v>
+      </c>
+      <c r="DQ9" s="13">
+        <v>2021</v>
       </c>
       <c r="DU9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="DY9" t="s">
         <v>311</v>
       </c>
       <c r="EC9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="EG9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="EK9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="EO9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="ES9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="EW9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="FA9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="FI9" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="FM9" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="FM9" s="13" t="s">
-        <v>421</v>
+      <c r="FQ9" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="FU9" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="FY9" s="13" t="s">
+        <v>455</v>
+      </c>
+      <c r="HO9" s="13" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="10" spans="1:303" x14ac:dyDescent="0.25">
+      <c r="BA10" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="BI10" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="BQ10" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="DQ10" s="13">
+        <v>2017</v>
+      </c>
+      <c r="EC10" t="s">
+        <v>471</v>
+      </c>
+      <c r="FQ10" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="FU10" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="FY10" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="HO10" s="13" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="11" spans="1:303" x14ac:dyDescent="0.25">
+      <c r="BA11" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="BI11" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="BQ11" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="DQ11" s="13">
+        <v>2017</v>
+      </c>
+      <c r="EC11" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="FQ11" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="FU11" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="FY11" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="HO11" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="12" spans="1:303" x14ac:dyDescent="0.25">
+      <c r="BA12" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="BI12" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="BQ12" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="DQ12" s="13">
+        <v>2017</v>
+      </c>
+      <c r="EC12" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="FQ12" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="FU12" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="FY12" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="HO12" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="13" spans="1:303" x14ac:dyDescent="0.25">
+      <c r="BA13" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="BI13" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="BQ13" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="DQ13" s="13">
+        <v>2017</v>
+      </c>
+      <c r="EC13" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="FQ13" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="FU13" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="FY13" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="HO13" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="14" spans="1:303" x14ac:dyDescent="0.25">
+      <c r="BA14" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="BI14" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="BQ14" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="DQ14" s="13">
+        <v>2025</v>
+      </c>
+      <c r="EC14" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="FQ14" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="FU14" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="FY14" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="HO14" s="13" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:303" x14ac:dyDescent="0.25">
+      <c r="BA15" t="s">
+        <v>470</v>
+      </c>
+      <c r="BI15" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="BQ15" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="DQ15" s="13">
+        <v>2016</v>
+      </c>
+      <c r="EC15" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="FQ15" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="FU15" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="FY15" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="HO15" s="13" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:303" x14ac:dyDescent="0.25">
+      <c r="BA16" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="BI16" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="BQ16" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="DQ16" s="13">
+        <v>2016</v>
+      </c>
+      <c r="EC16" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="FQ16" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="FU16" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="FY16" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="HO16" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="17" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA17" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="BI17" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="BQ17" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="DQ17" s="13">
+        <v>2016</v>
+      </c>
+      <c r="EC17" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="HO17" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="18" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA18" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="BI18" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="BQ18" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EC18" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="HO18" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="HP18" s="13"/>
+    </row>
+    <row r="19" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA19" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="BI19" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BQ19" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EC19" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="HO19" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="HP19" s="13"/>
+    </row>
+    <row r="20" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA20" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="BI20" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BQ20" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EC20" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="HO20" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="HP20" s="13"/>
+    </row>
+    <row r="21" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA21" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="BI21" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="BQ21" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EC21" s="13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA22" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="BI22" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="BQ22" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EC22" s="13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="23" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA23" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="BI23" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="BQ23" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EC23" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="24" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA24" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="BI24" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="BQ24" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="EC24" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA25" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="BI25" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="BQ25" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EC25" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="26" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA26" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="BI26" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="BQ26" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EC26" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="27" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA27" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI27" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="BQ27" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="EC27" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BA28" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="BI28" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="BQ28" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="EC28" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="29" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BQ29" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="EC29" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="30" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BQ30" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EC30" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="31" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BQ31" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="EC31" s="13" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="32" spans="53:224" x14ac:dyDescent="0.25">
+      <c r="BQ32" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="33" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ33" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="34" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ34" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="35" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ35" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="36" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ36" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="37" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ37" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="38" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ38" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="39" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ39" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="40" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ40" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="41" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ41" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="42" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ42" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="43" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ43" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="44" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ44" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="45" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ45" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="46" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ46" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="47" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ47" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="48" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ48" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="49" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ49" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="50" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ50" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="51" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ51" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="52" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ52" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="53" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ53" s="13" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="54" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ54" s="13" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="55" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ55" s="13" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="56" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ56" s="13" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="57" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ57" s="13" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="58" spans="69:69" x14ac:dyDescent="0.25">
+      <c r="BQ58" s="13" t="s">
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -3295,5 +4308,109 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
+  <drawing r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1028" r:id="rId11" name="Control 4">
+          <controlPr defaultSize="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1028" r:id="rId11" name="Control 4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId13" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId13" name="Control 3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId14" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId14" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId15" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId15" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished CSV printing added new fixed graphs
</commit_message>
<xml_diff>
--- a/uploads/example_data.xlsx
+++ b/uploads/example_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="473">
   <si>
     <t>Customer ID</t>
   </si>
@@ -1440,6 +1440,9 @@
   </si>
   <si>
     <t>Alexandria</t>
+  </si>
+  <si>
+    <t>Assiut</t>
   </si>
 </sst>
 </file>
@@ -2046,8 +2049,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:KQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DI1" workbookViewId="0">
-      <selection activeCell="DQ3" sqref="DQ3"/>
+    <sheetView tabSelected="1" topLeftCell="DP9" workbookViewId="0">
+      <selection activeCell="EC34" sqref="EC34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3936,7 +3939,7 @@
         <v>2016</v>
       </c>
       <c r="EC16" s="13" t="s">
-        <v>310</v>
+        <v>471</v>
       </c>
       <c r="FQ16" s="13" t="s">
         <v>435</v>
@@ -3965,7 +3968,7 @@
         <v>2016</v>
       </c>
       <c r="EC17" s="13" t="s">
-        <v>310</v>
+        <v>471</v>
       </c>
       <c r="HO17" t="s">
         <v>466</v>
@@ -3982,7 +3985,7 @@
         <v>325</v>
       </c>
       <c r="EC18" s="13" t="s">
-        <v>310</v>
+        <v>471</v>
       </c>
       <c r="HO18" s="13" t="s">
         <v>466</v>
@@ -4164,6 +4167,9 @@
     <row r="32" spans="53:224" x14ac:dyDescent="0.25">
       <c r="BQ32" s="13" t="s">
         <v>325</v>
+      </c>
+      <c r="EC32" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="33" spans="69:69" x14ac:dyDescent="0.25">
@@ -4313,8 +4319,58 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId11" name="Control 4">
+        <control shapeId="1025" r:id="rId11" name="Control 1">
           <controlPr defaultSize="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId11" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId13" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>222</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId13" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId15" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId14">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>222</xdr:col>
@@ -4333,13 +4389,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId11" name="Control 4"/>
+        <control shapeId="1027" r:id="rId15" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId13" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId12">
+        <control shapeId="1028" r:id="rId16" name="Control 4">
+          <controlPr defaultSize="0" r:id="rId14">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>222</xdr:col>
@@ -4358,57 +4414,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId13" name="Control 3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId14" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>222</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>222</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1026" r:id="rId14" name="Control 2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId15" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>222</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>222</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1025" r:id="rId15" name="Control 1"/>
+        <control shapeId="1028" r:id="rId16" name="Control 4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>